<commit_message>
fixed psa param template
</commit_message>
<xml_diff>
--- a/static/Course_Modularization/Sensitivity analysis/param template/param 3-state.xlsx
+++ b/static/Course_Modularization/Sensitivity analysis/param template/param 3-state.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinekrijkamp/Documents/GitHub/Course-Modularization/static/Course_Modularization/Sensitivity analysis/param template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Yang\Desktop\GitHub local\Course-Modularization\static\Course_Modularization\Sensitivity analysis\param template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAE9B89-7C68-ED47-B6BA-DCBA7073161B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A86A16F-25ED-40C0-8E01-87599647A4D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="0" windowWidth="24600" windowHeight="16000" xr2:uid="{6119A56A-EAB1-154D-9078-6C830EF23C18}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{6119A56A-EAB1-154D-9078-6C830EF23C18}"/>
   </bookViews>
   <sheets>
     <sheet name="param" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="51">
   <si>
     <t>normal</t>
   </si>
@@ -136,15 +136,9 @@
     <t>utility</t>
   </si>
   <si>
-    <t>49.5</t>
-  </si>
-  <si>
     <t>sigma</t>
   </si>
   <si>
-    <t>0.04</t>
-  </si>
-  <si>
     <t>lower_limit</t>
   </si>
   <si>
@@ -154,18 +148,6 @@
     <t>triangle</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>22.4</t>
-  </si>
-  <si>
-    <t>12.5</t>
-  </si>
-  <si>
     <t>par1</t>
   </si>
   <si>
@@ -197,34 +179,16 @@
   </si>
   <si>
     <t>c_trtB</t>
-  </si>
-  <si>
-    <t>201.6</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>6.67</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>0.0015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,18 +231,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -300,7 +270,7 @@
     <tableColumn id="3" xr3:uid="{B4ACDF6F-5578-4F46-9F1E-F32D5CFB6F05}" name="distribution"/>
     <tableColumn id="7" xr3:uid="{F9FD1E79-3AEF-444D-A7ED-979F37978BDC}" name="par1"/>
     <tableColumn id="8" xr3:uid="{5C1533D0-DCB5-BB49-BEED-5E4B8B968375}" name="par2"/>
-    <tableColumn id="4" xr3:uid="{BDC1362D-A7E2-464A-89E1-7CF89DF46355}" name="par3"/>
+    <tableColumn id="4" xr3:uid="{BDC1362D-A7E2-464A-89E1-7CF89DF46355}" name="par3" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{7F0D6C5E-02C2-9B45-AE2F-B6271464F30E}" name="type par1"/>
     <tableColumn id="6" xr3:uid="{47A54D96-DE19-434E-8F5A-C97CFE4FE106}" name="type par2"/>
     <tableColumn id="9" xr3:uid="{F656A381-BB2B-CC42-87A9-E343A0C8FCBF}" name="type par3"/>
@@ -611,21 +581,21 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.19921875" customWidth="1"/>
+    <col min="3" max="3" width="12.796875" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -635,34 +605,34 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -670,13 +640,13 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="D2" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E2" s="5">
         <v>24</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="5">
         <v>450</v>
       </c>
       <c r="G2" t="s">
@@ -689,9 +659,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -699,13 +669,13 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="D3" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="E3" s="5">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5">
         <v>368</v>
       </c>
       <c r="G3" t="s">
@@ -718,9 +688,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -728,13 +698,13 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="5">
         <v>16</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>767</v>
       </c>
       <c r="G4" t="s">
@@ -747,7 +717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -757,13 +727,13 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="5">
         <v>4</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <v>391</v>
       </c>
       <c r="G5" t="s">
@@ -776,7 +746,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -786,14 +756,14 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>57</v>
+      <c r="D6" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>22.4</v>
+      </c>
+      <c r="F6" s="5">
+        <v>201.6</v>
       </c>
       <c r="G6" t="s">
         <v>15</v>
@@ -805,12 +775,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -820,13 +790,13 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="5">
         <v>400</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
         <v>16</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="5">
         <v>25</v>
       </c>
       <c r="G8" t="s">
@@ -839,7 +809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -849,13 +819,13 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="5">
         <v>1000</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>100</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <v>10</v>
       </c>
       <c r="G9" t="s">
@@ -868,7 +838,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -878,18 +848,18 @@
       <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="5">
         <v>0</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -897,14 +867,14 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="5">
         <v>800</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="5">
         <v>64</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
+      <c r="F11" s="5">
+        <v>12.5</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
@@ -916,9 +886,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -926,14 +896,14 @@
       <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="5">
         <v>225</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="5">
         <v>225</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>61</v>
+      <c r="F12" s="5">
+        <v>6.67</v>
       </c>
       <c r="G12" t="s">
         <v>15</v>
@@ -945,12 +915,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -960,14 +930,14 @@
       <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="5">
         <v>1</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>63</v>
+      <c r="E14" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1.5E-3</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
@@ -979,7 +949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -989,14 +959,14 @@
       <c r="C15" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>36</v>
+      <c r="D15" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="5">
+        <v>49.5</v>
+      </c>
+      <c r="F15" s="5">
+        <v>49.5</v>
       </c>
       <c r="G15" t="s">
         <v>15</v>
@@ -1008,7 +978,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1018,16 +988,16 @@
       <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="5">
         <v>0</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
       <c r="G16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2">
       <c r="B31" t="s">
         <v>21</v>
       </c>
@@ -1066,9 +1036,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1079,7 +1049,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1095,7 +1065,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1111,15 +1081,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16.8">
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1127,7 +1097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1135,7 +1105,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1143,27 +1113,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="B10" t="s">
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="C11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="C12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on PSA template
</commit_message>
<xml_diff>
--- a/static/Course_Modularization/Sensitivity analysis/param template/param 3-state.xlsx
+++ b/static/Course_Modularization/Sensitivity analysis/param template/param 3-state.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Yang\Desktop\GitHub local\Course-Modularization\static\Course_Modularization\Sensitivity analysis\param template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinekrijkamp/Documents/GitHub/Course-Modularization/static/Course_Modularization/Sensitivity analysis/param template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A86A16F-25ED-40C0-8E01-87599647A4D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC40D4C6-5CFA-524F-9172-4F51AB99B9EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{6119A56A-EAB1-154D-9078-6C830EF23C18}"/>
+    <workbookView xWindow="920" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{6119A56A-EAB1-154D-9078-6C830EF23C18}"/>
   </bookViews>
   <sheets>
     <sheet name="param" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
   <si>
     <t>normal</t>
   </si>
@@ -40,15 +40,9 @@
     <t>gamma</t>
   </si>
   <si>
-    <t>weibull</t>
-  </si>
-  <si>
     <t>uniform</t>
   </si>
   <si>
-    <t xml:space="preserve">dirichlet </t>
-  </si>
-  <si>
     <t>parameter</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>shape2</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>c_D</t>
   </si>
   <si>
@@ -179,16 +170,16 @@
   </si>
   <si>
     <t>c_trtB</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,7 +228,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -581,61 +572,61 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -650,21 +641,21 @@
         <v>450</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -679,21 +670,21 @@
         <v>368</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -708,21 +699,21 @@
         <v>767</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -737,21 +728,21 @@
         <v>391</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -766,26 +757,26 @@
         <v>201.6</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -800,21 +791,21 @@
         <v>25</v>
       </c>
       <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
         <v>15</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -829,24 +820,24 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>17</v>
       </c>
-      <c r="I9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5">
         <v>0</v>
@@ -854,15 +845,15 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -877,21 +868,21 @@
         <v>12.5</v>
       </c>
       <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
         <v>15</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>17</v>
       </c>
-      <c r="I11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -906,26 +897,26 @@
         <v>6.67</v>
       </c>
       <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
         <v>15</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>17</v>
       </c>
-      <c r="I12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -940,21 +931,21 @@
         <v>1.5E-3</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -969,24 +960,24 @@
         <v>49.5</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D16" s="5">
         <v>0</v>
@@ -994,12 +985,12 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1009,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8585BF0-6750-394F-9D1D-7BD53BE8844F}">
           <x14:formula1>
-            <xm:f>'distribution names'!$B$2:$B$10</xm:f>
+            <xm:f>'distribution names'!$B$2:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C17</xm:sqref>
         </x14:dataValidation>
@@ -1033,39 +1024,39 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1073,67 +1064,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>